<commit_message>
Update ORCA bisferrocene VACT
</commit_message>
<xml_diff>
--- a/Algorithm/Characteristics_Setting/bisfe4_ox_counterionOnThiol_orca/characteristics_data.xlsx
+++ b/Algorithm/Characteristics_Setting/bisfe4_ox_counterionOnThiol_orca/characteristics_data.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="5" rupBuild="21929"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="5" rupBuild="22026"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\scerpa\Algorithm\Characteristics_Setting\bisfe4_ox_counterionOnThiol_orca\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{FDA907F1-8C7F-486E-A1EB-2D5323D5FC40}" xr6:coauthVersionLast="44" xr6:coauthVersionMax="44" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{EE98293B-4D81-42D3-8040-09608EF6A62A}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10560" tabRatio="500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="28680" yWindow="-120" windowWidth="29040" windowHeight="15990" tabRatio="500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Foglio1" sheetId="1" r:id="rId1"/>
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="6" uniqueCount="6">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="10" uniqueCount="10">
   <si>
     <t>File Name</t>
   </si>
@@ -31,13 +31,25 @@
     <t># Vin Values</t>
   </si>
   <si>
-    <t>ck1.txt</t>
-  </si>
-  <si>
-    <t>ck2.txt</t>
-  </si>
-  <si>
-    <t>ck3.txt</t>
+    <t>ck20.txt</t>
+  </si>
+  <si>
+    <t>ck15.txt</t>
+  </si>
+  <si>
+    <t>ck10.txt</t>
+  </si>
+  <si>
+    <t>ck00.txt</t>
+  </si>
+  <si>
+    <t>ckm10.txt</t>
+  </si>
+  <si>
+    <t>ckm15.txt</t>
+  </si>
+  <si>
+    <t>ckm20.txt</t>
   </si>
 </sst>
 </file>
@@ -349,10 +361,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:C4"/>
+  <dimension ref="A1:C8"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C2" sqref="C2"/>
+      <selection activeCell="H18" sqref="H18"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -379,10 +391,10 @@
         <v>3</v>
       </c>
       <c r="B2">
-        <v>-2</v>
+        <v>2</v>
       </c>
       <c r="C2">
-        <v>39</v>
+        <v>24</v>
       </c>
     </row>
     <row r="3" spans="1:3" x14ac:dyDescent="0.35">
@@ -390,10 +402,10 @@
         <v>4</v>
       </c>
       <c r="B3">
-        <v>0</v>
+        <v>1.5</v>
       </c>
       <c r="C3">
-        <v>39</v>
+        <v>24</v>
       </c>
     </row>
     <row r="4" spans="1:3" x14ac:dyDescent="0.35">
@@ -401,9 +413,53 @@
         <v>5</v>
       </c>
       <c r="B4">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="C4">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="5" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A5" t="s">
+        <v>6</v>
+      </c>
+      <c r="B5">
+        <v>0</v>
+      </c>
+      <c r="C5">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="6" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A6" t="s">
+        <v>7</v>
+      </c>
+      <c r="B6">
+        <v>-1</v>
+      </c>
+      <c r="C6">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="7" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A7" t="s">
+        <v>8</v>
+      </c>
+      <c r="B7">
+        <v>-1.5</v>
+      </c>
+      <c r="C7">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="8" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A8" t="s">
+        <v>9</v>
+      </c>
+      <c r="B8">
+        <v>-2</v>
+      </c>
+      <c r="C8">
         <v>24</v>
       </c>
     </row>

</xml_diff>